<commit_message>
Update sample file with correct email format
</commit_message>
<xml_diff>
--- a/apps/api/src/assets/sample/import-class-sample.xlsx
+++ b/apps/api/src/assets/sample/import-class-sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuuNguyen\OneDrive - Đại học FPT- FPT University\Desktop\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoadtran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75C3E38-CCD6-4173-AB80-904A87090594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A28D85-814D-9E47-A989-08FD7DA6B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>email</t>
   </si>
@@ -33,34 +33,16 @@
     <t>fullName</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
-    <t>student1</t>
-  </si>
-  <si>
-    <t>student2</t>
-  </si>
-  <si>
-    <t>student3</t>
-  </si>
-  <si>
-    <t>student4</t>
-  </si>
-  <si>
-    <t>student5</t>
+    <t>minhntse140988@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Tran Nhat Minh</t>
+  </si>
+  <si>
+    <t>buunqse140936@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Nguyen Quoc Buu</t>
   </si>
 </sst>
 </file>
@@ -395,19 +377,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,55 +397,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DFCBD23A-0E11-48C2-8EC6-02DBA95C9745}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{28E17A61-1E07-4967-BBD5-3B32059C13EE}"/>
-    <hyperlink ref="A3:A6" r:id="rId3" display="test1@gmail.com" xr:uid="{C10DD66B-2EF2-485E-B6B5-726ACB49C9A3}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{4D3AEA71-B6A5-4068-8D59-4687888AEA3C}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{CFDD5312-C4FF-4A0E-8F33-53DCBBA91C78}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{E8CCB8F5-3FDF-4060-B22C-EF750F80F8AF}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{76822665-D1C8-46B7-A815-93D7656C8112}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>